<commit_message>
Added source for vestas total capacity and added new numbers
</commit_message>
<xml_diff>
--- a/Energy of Wind/Scripts/ger-pol-fin-research.xlsx
+++ b/Energy of Wind/Scripts/ger-pol-fin-research.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9eea8fa18fefeb31/Documents/GitHub/Team-27/Energy of Wind/Scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C69DAC39-5CB4-4B9F-984C-5F214D89A85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F354273C-F3F9-DE4F-90F2-CD859483AE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15860" yWindow="2380" windowWidth="25580" windowHeight="13780" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ger-pol-fin-research" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="19">
   <si>
     <t>Year</t>
   </si>
@@ -83,7 +95,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -924,21 +936,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I11"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="14" width="19.54296875" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="14" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -982,7 +994,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2017</v>
       </c>
@@ -1000,14 +1012,14 @@
         <v>0.10924522472420624</v>
       </c>
       <c r="I2" s="3">
-        <f>G2/G30</f>
+        <f>G2/G35</f>
         <v>0.10815041381792012</v>
       </c>
       <c r="L2">
         <v>4616</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1028,7 +1040,7 @@
         <v>0.11961216394887615</v>
       </c>
       <c r="I3" s="3">
-        <f>G3/G31</f>
+        <f>G3/G36</f>
         <v>0.11529311809685641</v>
       </c>
       <c r="J3">
@@ -1047,7 +1059,7 @@
         <v>3762</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2019</v>
       </c>
@@ -1068,7 +1080,7 @@
         <v>0.12510828280135936</v>
       </c>
       <c r="I4" s="3">
-        <f>G4/G32</f>
+        <f>G4/G37</f>
         <v>0.12368247694334651</v>
       </c>
       <c r="J4">
@@ -1087,7 +1099,7 @@
         <v>4389</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -1108,7 +1120,7 @@
         <v>9.958243534482758E-2</v>
       </c>
       <c r="I5" s="3">
-        <f>G5/G33</f>
+        <f>G5/G38</f>
         <v>0.11813678491530841</v>
       </c>
       <c r="J5">
@@ -1127,7 +1139,7 @@
         <v>4710</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -1148,7 +1160,7 @@
         <v>9.4723418224977582E-2</v>
       </c>
       <c r="I6" s="3">
-        <f>G6/G34</f>
+        <f>G6/G39</f>
         <v>0.11714553404122423</v>
       </c>
       <c r="J6">
@@ -1167,7 +1179,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2017</v>
       </c>
@@ -1185,7 +1197,7 @@
         <v>1.8992057866710283E-2</v>
       </c>
       <c r="I7" s="3">
-        <f>G7/G36</f>
+        <f>G7/G41</f>
         <v>0.16335782397999063</v>
       </c>
       <c r="J7">
@@ -1204,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -1222,7 +1234,7 @@
         <v>1.8422212428382548E-2</v>
       </c>
       <c r="I8" s="3">
-        <f>G8/G37</f>
+        <f>G8/G42</f>
         <v>0.17820600272851295</v>
       </c>
       <c r="J8">
@@ -1241,7 +1253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2019</v>
       </c>
@@ -1259,7 +1271,7 @@
         <v>1.7541813820217231E-2</v>
       </c>
       <c r="I9" s="3">
-        <f>G9/G38</f>
+        <f>G9/G43</f>
         <v>0.17796180496873415</v>
       </c>
       <c r="J9">
@@ -1278,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2020</v>
       </c>
@@ -1296,7 +1308,7 @@
         <v>1.5611530172413794E-2</v>
       </c>
       <c r="I10" s="3">
-        <f>G10/G39</f>
+        <f>G10/G44</f>
         <v>0.17523435137586937</v>
       </c>
       <c r="J10">
@@ -1315,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -1333,7 +1345,7 @@
         <v>1.6376469399866159E-2</v>
       </c>
       <c r="I11" s="3">
-        <f>G11/G40</f>
+        <f>G11/G45</f>
         <v>0.18226531759415401</v>
       </c>
       <c r="J11">
@@ -1352,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2017</v>
       </c>
@@ -1368,7 +1380,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2018</v>
       </c>
@@ -1383,7 +1395,7 @@
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2019</v>
       </c>
@@ -1398,7 +1410,7 @@
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2020</v>
       </c>
@@ -1413,7 +1425,7 @@
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2021</v>
       </c>
@@ -1428,7 +1440,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2016</v>
       </c>
@@ -1448,7 +1460,7 @@
         <v>0.11600000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2017</v>
       </c>
@@ -1468,7 +1480,7 @@
         <v>0.152</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2018</v>
       </c>
@@ -1488,7 +1500,7 @@
         <v>0.123</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -1508,7 +1520,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2020</v>
       </c>
@@ -1528,7 +1540,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2021</v>
       </c>
@@ -1547,8 +1559,15 @@
       <c r="F22" s="1">
         <v>3.5999999999999997E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G22">
+        <v>16438</v>
+      </c>
+      <c r="I22" s="3">
+        <f>G22/G39</f>
+        <v>0.25668332292317303</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2016</v>
       </c>
@@ -1568,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2017</v>
       </c>
@@ -1588,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2018</v>
       </c>
@@ -1608,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -1628,7 +1647,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2020</v>
       </c>
@@ -1648,7 +1667,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2021</v>
       </c>
@@ -1667,80 +1686,92 @@
       <c r="F28" s="1">
         <v>4.4999999999999998E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G28">
+        <v>3559</v>
+      </c>
+      <c r="I28" s="3">
+        <f>G28/G45</f>
+        <v>0.50014052838673417</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
+        <v>2017</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29">
+        <v>8779</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2018</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30">
+        <v>10847</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2019</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31">
+        <v>12884</v>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2020</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32">
+        <v>17212</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2021</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33">
+        <v>16594</v>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>2016</v>
-      </c>
-      <c r="B29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29">
-        <v>49430</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>2017</v>
-      </c>
-      <c r="B30" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30">
-        <v>55580</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>2018</v>
-      </c>
-      <c r="B31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31">
-        <v>58850</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>2019</v>
-      </c>
-      <c r="B32" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32">
-        <v>60720</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>2020</v>
-      </c>
-      <c r="B33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33">
-        <v>62580</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>2021</v>
       </c>
       <c r="B34" t="s">
         <v>16</v>
@@ -1749,82 +1780,82 @@
         <v>13</v>
       </c>
       <c r="G34">
-        <v>64040</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+        <v>49430</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B35" t="s">
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35">
-        <v>5782</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+        <v>55580</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B36" t="s">
         <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G36">
-        <v>6397</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+        <v>58850</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B37" t="s">
         <v>16</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G37">
-        <v>5864</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+        <v>60720</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B38" t="s">
         <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G38">
-        <v>5917</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+        <v>62580</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B39" t="s">
         <v>16</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G39">
-        <v>6614</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+        <v>64040</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B40" t="s">
         <v>16</v>
@@ -1833,6 +1864,76 @@
         <v>14</v>
       </c>
       <c r="G40">
+        <v>5782</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2017</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41">
+        <v>6397</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2018</v>
+      </c>
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42">
+        <v>5864</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2019</v>
+      </c>
+      <c r="B43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43">
+        <v>5917</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2020</v>
+      </c>
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44">
+        <v>6614</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2021</v>
+      </c>
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45">
         <v>7116</v>
       </c>
     </row>
@@ -1843,22 +1944,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1875,7 +1976,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2017</v>
       </c>
@@ -1892,7 +1993,7 @@
         <v>0.10815041381792012</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1909,7 +2010,7 @@
         <v>0.11529311809685641</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2019</v>
       </c>
@@ -1926,7 +2027,7 @@
         <v>0.12368247694334651</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -1943,7 +2044,7 @@
         <v>0.11813678491530841</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -1960,7 +2061,7 @@
         <v>0.11714553404122423</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2017</v>
       </c>
@@ -1977,7 +2078,7 @@
         <v>0.16335782397999063</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -1994,7 +2095,7 @@
         <v>0.17820600272851295</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2019</v>
       </c>
@@ -2011,7 +2112,7 @@
         <v>0.17796180496873415</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2020</v>
       </c>
@@ -2028,7 +2129,7 @@
         <v>0.17523435137586937</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -2043,6 +2144,152 @@
       </c>
       <c r="E11" s="3">
         <v>0.18226531759415401</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2017</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2018</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2019</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2020</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2021</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.25668332292317303</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2017</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2018</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2019</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2020</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2021</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="1">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.50014052838673417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>